<commit_message>
correcting rogue entry in simIII
</commit_message>
<xml_diff>
--- a/data/pfc2019/RMSonlyvsTime2018-DSA2000-CWOptimized-SimulationIII.xlsx
+++ b/data/pfc2019/RMSonlyvsTime2018-DSA2000-CWOptimized-SimulationIII.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylosr8/Research/repos/pta_simulations/data/pfc2019/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A45730A-81F5-624D-8845-B642759F747E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38100" yWindow="0" windowWidth="27920" windowHeight="40360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -825,8 +837,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2384,14 +2396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="J284" sqref="J284"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" customWidth="1"/>
@@ -5627,7 +5639,7 @@
         <v>0.185871854</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -5656,7 +5668,7 @@
         <v>0.18873558400000001</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -5685,7 +5697,7 @@
         <v>0.20622227000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -5714,7 +5726,7 @@
         <v>0.20783120399999999</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -5743,7 +5755,7 @@
         <v>0.33402543800000001</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -5772,7 +5784,7 @@
         <v>0.34920448799999998</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -5801,7 +5813,7 @@
         <v>0.375881248</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -5830,7 +5842,7 @@
         <v>0.39735119200000002</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>92</v>
       </c>
@@ -5852,12 +5864,8 @@
       <c r="G105">
         <v>0.35437809199999998</v>
       </c>
-      <c r="K105">
-        <f>G105/2</f>
-        <v>0.17718904599999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11">
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -5880,7 +5888,7 @@
         <v>0.360257406</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -5903,7 +5911,7 @@
         <v>0.36101279800000002</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -5926,7 +5934,7 @@
         <v>0.36795630200000001</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -5949,7 +5957,7 @@
         <v>0.38229138400000001</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -5972,7 +5980,7 @@
         <v>0.39159143600000001</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>113</v>
       </c>
@@ -5995,7 +6003,7 @@
         <v>0.421543838</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>114</v>
       </c>

</xml_diff>